<commit_message>
remove some comments in spark scripts
</commit_message>
<xml_diff>
--- a/UoM_MapReduce-vs-Spark/Spark/results and screenshots/execution-times.xlsx
+++ b/UoM_MapReduce-vs-Spark/Spark/results and screenshots/execution-times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msc\06.Semester-07\229412h-emr-lab\UoM_MapReduce-vs-Spark\Spark\results and screenshots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198AE60F-0176-4D2B-8E0B-882C9136A499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12226FD1-6125-4E2C-9A9D-00BA61D990CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7C55F0A3-E3A0-46D8-B43C-CB936204491A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Year wise carrier delay from 2003-2010</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Execution Time (Seconds)</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E33B63-574D-466E-BFD4-D14BDAC2922B}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,6 +503,15 @@
         <v>30</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f>AVERAGE(C2:C6)</f>
+        <v>33.200000000000003</v>
+      </c>
+    </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
@@ -543,6 +555,15 @@
         <v>46</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C9:C13)</f>
+        <v>31.6</v>
+      </c>
+    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>3</v>
@@ -586,6 +607,15 @@
         <v>28</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGE(C16:C20)</f>
+        <v>28.4</v>
+      </c>
+    </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>4</v>
@@ -629,6 +659,15 @@
         <v>28</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(C23:C27)</f>
+        <v>27.6</v>
+      </c>
+    </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>5</v>
@@ -670,6 +709,15 @@
       </c>
       <c r="C34">
         <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <f>AVERAGE(C30:C34)</f>
+        <v>27.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>